<commit_message>
fix domain in framework
</commit_message>
<xml_diff>
--- a/docs/tables/MlSecOps_Process_Framework.xlsx
+++ b/docs/tables/MlSecOps_Process_Framework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arsemenov\cyberorda.github.io\docs\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C011F-6039-47BA-A605-A0FAA7405723}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA87B7A8-4E0F-47AB-9B22-261F4D6030E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="6330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="205">
   <si>
     <t>Шифрование данных при хранении и передаче</t>
   </si>
@@ -680,6 +680,12 @@
       <t xml:space="preserve">
 Такой артефакт необходимо сделать обязательным к исполнению и осуществлять контроль за выполнением всех изложенных в нём требований.</t>
     </r>
+  </si>
+  <si>
+    <t>Разработка ML модели</t>
+  </si>
+  <si>
+    <t>Домен описывает практики, связанные с разработкой модели.</t>
   </si>
 </sst>
 </file>
@@ -862,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -922,6 +928,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -940,37 +976,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1256,8 +1265,8 @@
   <dimension ref="A1:F318"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="78" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="A1:F79"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1293,16 +1302,16 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="367" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1313,10 +1322,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="218.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="30"/>
       <c r="E3" s="15" t="s">
         <v>59</v>
       </c>
@@ -1325,10 +1334,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="173" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="15" t="s">
         <v>71</v>
       </c>
@@ -1337,12 +1346,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="128" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="24" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="31" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="16" t="s">
@@ -1353,10 +1362,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="128" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="12" t="s">
         <v>60</v>
       </c>
@@ -1365,10 +1374,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="128" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="28"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="22"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="32"/>
       <c r="E7" s="12" t="s">
         <v>78</v>
       </c>
@@ -1377,10 +1386,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="209.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="28"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="22"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="32"/>
       <c r="E8" s="16" t="s">
         <v>57</v>
       </c>
@@ -1389,10 +1398,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="32"/>
       <c r="E9" s="17" t="s">
         <v>36</v>
       </c>
@@ -1401,12 +1410,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="28"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="31" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -1417,10 +1426,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="229" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="32"/>
       <c r="E11" s="12" t="s">
         <v>40</v>
       </c>
@@ -1429,10 +1438,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="115" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="33"/>
       <c r="E12" s="12" t="s">
         <v>41</v>
       </c>
@@ -1441,12 +1450,12 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="192" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="30" t="s">
         <v>62</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -1457,10 +1466,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A14" s="28"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="32"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="12" t="s">
         <v>64</v>
       </c>
@@ -1469,12 +1478,12 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="28"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="30" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -1485,10 +1494,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="120.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="18" t="s">
         <v>25</v>
       </c>
@@ -1497,12 +1506,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="25" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="31" t="s">
         <v>101</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -1513,10 +1522,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="12" t="s">
         <v>0</v>
       </c>
@@ -1525,10 +1534,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="191" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="28"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="12" t="s">
         <v>42</v>
       </c>
@@ -1537,10 +1546,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="249.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="28"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="22"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="12" t="s">
         <v>66</v>
       </c>
@@ -1549,10 +1558,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="169.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="12" t="s">
         <v>67</v>
       </c>
@@ -1561,10 +1570,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1" ht="225" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="23"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="12" t="s">
         <v>43</v>
       </c>
@@ -1573,16 +1582,16 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="30" t="s">
         <v>91</v>
       </c>
       <c r="E23" s="19" t="s">
@@ -1593,10 +1602,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="28"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="12" t="s">
         <v>92</v>
       </c>
@@ -1605,10 +1614,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="64" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="28"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="32"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="12" t="s">
         <v>7</v>
       </c>
@@ -1617,12 +1626,12 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="31" t="s">
+      <c r="A26" s="23"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="30" t="s">
         <v>31</v>
       </c>
       <c r="E26" s="12" t="s">
@@ -1633,10 +1642,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="28"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1645,10 +1654,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="28"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1657,10 +1666,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A29" s="28"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="32"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="12" t="s">
         <v>109</v>
       </c>
@@ -1669,12 +1678,12 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="28"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="31" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="30" t="s">
         <v>90</v>
       </c>
       <c r="E30" s="12" t="s">
@@ -1685,10 +1694,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A31" s="28"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="12" t="s">
         <v>112</v>
       </c>
@@ -1697,10 +1706,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="162.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="28"/>
-      <c r="B32" s="35"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="12" t="s">
         <v>116</v>
       </c>
@@ -1709,10 +1718,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A33" s="28"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="12" t="s">
         <v>33</v>
       </c>
@@ -1721,10 +1730,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A34" s="28"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="12" t="s">
         <v>9</v>
       </c>
@@ -1733,12 +1742,12 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="24" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="31" t="s">
         <v>194</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -1749,10 +1758,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A36" s="28"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="22"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="12" t="s">
         <v>11</v>
       </c>
@@ -1761,10 +1770,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A37" s="28"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="22"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="12" t="s">
         <v>87</v>
       </c>
@@ -1773,10 +1782,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A38" s="28"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="23"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="33"/>
       <c r="E38" s="12" t="s">
         <v>80</v>
       </c>
@@ -1785,12 +1794,12 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="28"/>
-      <c r="B39" s="35"/>
-      <c r="C39" s="31" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="30" t="s">
         <v>44</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -1801,10 +1810,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A40" s="28"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="12" t="s">
         <v>82</v>
       </c>
@@ -1813,10 +1822,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A41" s="28"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="12" t="s">
         <v>10</v>
       </c>
@@ -1825,10 +1834,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A42" s="28"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="12" t="s">
         <v>84</v>
       </c>
@@ -1837,10 +1846,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A43" s="28"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="32"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="12" t="s">
         <v>83</v>
       </c>
@@ -1849,10 +1858,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="138.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="28"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="12" t="s">
         <v>26</v>
       </c>
@@ -1861,12 +1870,16 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A45" s="28"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="25" t="s">
+      <c r="A45" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="32" t="s">
         <v>195</v>
       </c>
       <c r="E45" s="20" t="s">
@@ -1877,10 +1890,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="22"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="20" t="s">
         <v>125</v>
       </c>
@@ -1889,10 +1902,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A47" s="28"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="22"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="12" t="s">
         <v>123</v>
       </c>
@@ -1901,10 +1914,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A48" s="28"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="23"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="33"/>
       <c r="E48" s="20" t="s">
         <v>122</v>
       </c>
@@ -1913,12 +1926,12 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A49" s="28"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="24" t="s">
+      <c r="A49" s="37"/>
+      <c r="B49" s="38"/>
+      <c r="C49" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="D49" s="21" t="s">
+      <c r="D49" s="31" t="s">
         <v>196</v>
       </c>
       <c r="E49" s="12" t="s">
@@ -1929,10 +1942,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A50" s="28"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="22"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="12" t="s">
         <v>126</v>
       </c>
@@ -1941,10 +1954,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A51" s="28"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="22"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="38"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="12" t="s">
         <v>183</v>
       </c>
@@ -1953,10 +1966,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="140" x14ac:dyDescent="0.35">
-      <c r="A52" s="28"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="22"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="12" t="s">
         <v>127</v>
       </c>
@@ -1965,10 +1978,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="126" x14ac:dyDescent="0.35">
-      <c r="A53" s="28"/>
-      <c r="B53" s="35"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="22"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="38"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="32"/>
       <c r="E53" s="12" t="s">
         <v>128</v>
       </c>
@@ -1977,10 +1990,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="140" x14ac:dyDescent="0.35">
-      <c r="A54" s="28"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="22"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="12" t="s">
         <v>86</v>
       </c>
@@ -1989,10 +2002,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="42" x14ac:dyDescent="0.35">
-      <c r="A55" s="28"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="22"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="12" t="s">
         <v>129</v>
       </c>
@@ -2001,10 +2014,10 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A56" s="28"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="22"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="12" t="s">
         <v>45</v>
       </c>
@@ -2013,10 +2026,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A57" s="28"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="23"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="33"/>
       <c r="E57" s="12" t="s">
         <v>130</v>
       </c>
@@ -2025,12 +2038,12 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A58" s="28"/>
-      <c r="B58" s="35"/>
-      <c r="C58" s="24" t="s">
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="D58" s="31" t="s">
         <v>197</v>
       </c>
       <c r="E58" s="12" t="s">
@@ -2041,10 +2054,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A59" s="28"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="22"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="12" t="s">
         <v>133</v>
       </c>
@@ -2053,10 +2066,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A60" s="28"/>
-      <c r="B60" s="35"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="22"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="32"/>
       <c r="E60" s="12" t="s">
         <v>135</v>
       </c>
@@ -2065,10 +2078,10 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A61" s="28"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="22"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="32"/>
       <c r="E61" s="12" t="s">
         <v>134</v>
       </c>
@@ -2077,10 +2090,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A62" s="33"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="23"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="33"/>
       <c r="E62" s="12" t="s">
         <v>46</v>
       </c>
@@ -2089,16 +2102,16 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A63" s="27" t="s">
+      <c r="A63" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="29" t="s">
+      <c r="B63" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="21" t="s">
+      <c r="D63" s="31" t="s">
         <v>198</v>
       </c>
       <c r="E63" s="12" t="s">
@@ -2109,10 +2122,10 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="126" x14ac:dyDescent="0.35">
-      <c r="A64" s="28"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="22"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="32"/>
       <c r="E64" s="12" t="s">
         <v>142</v>
       </c>
@@ -2121,10 +2134,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A65" s="28"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="23"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="33"/>
       <c r="E65" s="12" t="s">
         <v>140</v>
       </c>
@@ -2133,12 +2146,12 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A66" s="28"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="31" t="s">
+      <c r="A66" s="23"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D66" s="21" t="s">
+      <c r="D66" s="31" t="s">
         <v>199</v>
       </c>
       <c r="E66" s="12" t="s">
@@ -2149,10 +2162,10 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A67" s="28"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="22"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="32"/>
       <c r="E67" s="12" t="s">
         <v>155</v>
       </c>
@@ -2161,10 +2174,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="70" x14ac:dyDescent="0.35">
-      <c r="A68" s="28"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="22"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="32"/>
       <c r="E68" s="12" t="s">
         <v>141</v>
       </c>
@@ -2173,10 +2186,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="126" x14ac:dyDescent="0.35">
-      <c r="A69" s="28"/>
-      <c r="B69" s="30"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="22"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="32"/>
       <c r="E69" s="12" t="s">
         <v>19</v>
       </c>
@@ -2185,10 +2198,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A70" s="28"/>
-      <c r="B70" s="30"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="23"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="33"/>
       <c r="E70" s="12" t="s">
         <v>20</v>
       </c>
@@ -2197,12 +2210,12 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A71" s="28"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="31" t="s">
+      <c r="A71" s="23"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="31" t="s">
         <v>200</v>
       </c>
       <c r="E71" s="12" t="s">
@@ -2213,10 +2226,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="112" x14ac:dyDescent="0.35">
-      <c r="A72" s="28"/>
-      <c r="B72" s="30"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="22"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="32"/>
       <c r="E72" s="12" t="s">
         <v>17</v>
       </c>
@@ -2225,10 +2238,10 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A73" s="28"/>
-      <c r="B73" s="30"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="22"/>
+      <c r="A73" s="23"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="32"/>
       <c r="E73" s="12" t="s">
         <v>161</v>
       </c>
@@ -2237,10 +2250,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="126" x14ac:dyDescent="0.35">
-      <c r="A74" s="28"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="22"/>
+      <c r="A74" s="23"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="32"/>
       <c r="E74" s="12" t="s">
         <v>160</v>
       </c>
@@ -2249,10 +2262,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="154" x14ac:dyDescent="0.35">
-      <c r="A75" s="28"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="22"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="12" t="s">
         <v>159</v>
       </c>
@@ -2261,10 +2274,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="84" x14ac:dyDescent="0.35">
-      <c r="A76" s="28"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="23"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="33"/>
       <c r="E76" s="12" t="s">
         <v>18</v>
       </c>
@@ -2273,12 +2286,12 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="140" x14ac:dyDescent="0.35">
-      <c r="A77" s="28"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="31" t="s">
+      <c r="A77" s="23"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D77" s="21" t="s">
+      <c r="D77" s="31" t="s">
         <v>201</v>
       </c>
       <c r="E77" s="12" t="s">
@@ -2289,10 +2302,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="154" x14ac:dyDescent="0.35">
-      <c r="A78" s="28"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="22"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="28"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="32"/>
       <c r="E78" s="12" t="s">
         <v>14</v>
       </c>
@@ -2301,10 +2314,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="98" x14ac:dyDescent="0.35">
-      <c r="A79" s="33"/>
-      <c r="B79" s="37"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="23"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="33"/>
       <c r="E79" s="12" t="s">
         <v>15</v>
       </c>
@@ -4225,19 +4238,19 @@
       <c r="F318" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="C77:C79"/>
-    <mergeCell ref="A23:A62"/>
-    <mergeCell ref="B23:B62"/>
-    <mergeCell ref="A63:A79"/>
-    <mergeCell ref="B63:B79"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="D71:D76"/>
+  <mergeCells count="44">
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="B2:B22"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
     <mergeCell ref="D77:D79"/>
     <mergeCell ref="C63:C65"/>
     <mergeCell ref="D26:D29"/>
@@ -4253,21 +4266,23 @@
     <mergeCell ref="D63:D65"/>
     <mergeCell ref="C58:C62"/>
     <mergeCell ref="D58:D62"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="A2:A22"/>
-    <mergeCell ref="B2:B22"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D5:D9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
     <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="D71:D76"/>
     <mergeCell ref="D45:D48"/>
     <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C77:C79"/>
+    <mergeCell ref="A63:A79"/>
+    <mergeCell ref="B63:B79"/>
+    <mergeCell ref="A23:A44"/>
+    <mergeCell ref="B23:B44"/>
+    <mergeCell ref="B45:B62"/>
+    <mergeCell ref="A45:A62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>